<commit_message>
update free spin permission file
</commit_message>
<xml_diff>
--- a/role_permission_files/FreeSpinPortal_RoleAndPermission_v0.1.xlsx
+++ b/role_permission_files/FreeSpinPortal_RoleAndPermission_v0.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.lou\DevOps\free_spin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ming.wong\git\rigi\sso_rws\role_permission_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>internal_external_role</t>
   </si>
@@ -63,18 +63,9 @@
     <t>create</t>
   </si>
   <si>
-    <t>change</t>
-  </si>
-  <si>
-    <t>promotions</t>
-  </si>
-  <si>
     <t>promotion</t>
   </si>
   <si>
-    <t>promotion_status</t>
-  </si>
-  <si>
     <t>Version Control</t>
   </si>
   <si>
@@ -103,6 +94,9 @@
   </si>
   <si>
     <t>account_manager</t>
+  </si>
+  <si>
+    <t>update_status</t>
   </si>
 </sst>
 </file>
@@ -185,14 +179,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -489,98 +483,98 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="C2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="7">
+        <v>18</v>
+      </c>
+      <c r="D4" s="6">
         <v>42331</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C5" s="3"/>
-      <c r="D5" s="7"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C6" s="3"/>
-      <c r="D6" s="7"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C7" s="3"/>
-      <c r="D7" s="7"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C8" s="3"/>
-      <c r="D8" s="7"/>
+      <c r="D8" s="6"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C9" s="3"/>
-      <c r="D9" s="7"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="8"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C10" s="3"/>
-      <c r="D10" s="7"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C11" s="3"/>
-      <c r="D11" s="7"/>
+      <c r="D11" s="6"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C12" s="3"/>
-      <c r="D12" s="7"/>
+      <c r="D12" s="6"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C13" s="3"/>
-      <c r="D13" s="7"/>
+      <c r="D13" s="6"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C14" s="3"/>
-      <c r="D14" s="7"/>
+      <c r="D14" s="6"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
@@ -603,7 +597,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,10 +635,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -652,7 +646,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
@@ -669,7 +663,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>4</v>
@@ -682,7 +676,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>4</v>
@@ -695,7 +689,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>4</v>
@@ -709,10 +703,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>4</v>

</xml_diff>